<commit_message>
Further work on Lab5. Still needs an abstract and conclusion. Very little qualitative information in this lab, in spite of it's saying that there should be.
</commit_message>
<xml_diff>
--- a/PHY431/Labs/Lab5_Data.xlsx
+++ b/PHY431/Labs/Lab5_Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Angle</t>
   </si>
@@ -67,6 +67,24 @@
   <si>
     <t>R^2</t>
   </si>
+  <si>
+    <t>=$B$2+$D$2 *(COS((A8+$A$2)*PI()/180)^2)</t>
+  </si>
+  <si>
+    <t>Enaught</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>Itot</t>
+  </si>
+  <si>
+    <t>pi/2</t>
+  </si>
+  <si>
+    <t>pi/4</t>
+  </si>
 </sst>
 </file>
 
@@ -101,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2724,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,6 +2787,11 @@
         <v>0.88</v>
       </c>
     </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
@@ -2796,7 +2820,7 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="C6">
-        <f>$B$2+$D$2 *(COS((A6+$A$2)*PI()/180)^2)</f>
+        <f t="shared" ref="C6:C23" si="0">$B$2+$D$2 *(COS((A6+$A$2)*PI()/180)^2)</f>
         <v>0.48930715155258475</v>
       </c>
       <c r="D6">
@@ -2815,14 +2839,14 @@
         <v>-85</v>
       </c>
       <c r="I6">
-        <f>$B$2+0.5*$D$2 *(1+COS((H6+$A$2)*2*PI()/180))</f>
+        <f t="shared" ref="I6:I23" si="1">$B$2+0.5*$D$2 *(1+COS((H6+$A$2)*2*PI()/180))</f>
         <v>0.48930715155258475</v>
       </c>
       <c r="K6">
         <v>-85</v>
       </c>
       <c r="L6">
-        <f>$B$2+$D$2 *(COS((K6+$A$2)*PI()/180)^2)</f>
+        <f t="shared" ref="L6:L23" si="2">$B$2+$D$2 *(COS((K6+$A$2)*PI()/180)^2)</f>
         <v>0.48930715155258475</v>
       </c>
     </row>
@@ -2834,29 +2858,29 @@
         <v>0.34</v>
       </c>
       <c r="C7">
-        <f>$B$2+$D$2 *(COS((A7+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.34103587704664795</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D23" si="0">(B7-C7)^2</f>
+        <f t="shared" ref="D7:D23" si="3">(B7-C7)^2</f>
         <v>1.0730412557720296E-6</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E23" si="1">(B7-$B$25)^2</f>
+        <f t="shared" ref="E7:E23" si="4">(B7-$B$25)^2</f>
         <v>3.2001234567901209E-2</v>
       </c>
       <c r="H7">
         <v>-75</v>
       </c>
       <c r="I7">
-        <f>$B$2+0.5*$D$2 *(1+COS((H7+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.34103587704664795</v>
       </c>
       <c r="K7">
         <v>-75</v>
       </c>
       <c r="L7">
-        <f>$B$2+$D$2 *(COS((K7+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.34103587704664795</v>
       </c>
     </row>
@@ -2872,25 +2896,25 @@
         <v>0.21435031699804108</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.2208800303435047E-7</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.2348456790123448E-2</v>
       </c>
       <c r="H8">
         <v>-65</v>
       </c>
       <c r="I8">
-        <f>$B$2+0.5*$D$2 *(1+COS((H8+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.21435031699804108</v>
       </c>
       <c r="K8">
         <v>-65</v>
       </c>
       <c r="L8">
-        <f>$B$2+$D$2 *(COS((K8+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.21435031699804108</v>
       </c>
     </row>
@@ -2902,29 +2926,29 @@
         <v>0.125</v>
       </c>
       <c r="C9">
-        <f>$B$2+$D$2 *(COS((A9+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.12453061962836645</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.2031793327484832E-7</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.15514845679012343</v>
       </c>
       <c r="H9">
         <v>-55</v>
       </c>
       <c r="I9">
-        <f>$B$2+0.5*$D$2 *(1+COS((H9+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.12453061962836645</v>
       </c>
       <c r="K9">
         <v>-55</v>
       </c>
       <c r="L9">
-        <f>$B$2+$D$2 *(COS((K9+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.12453061962836645</v>
       </c>
     </row>
@@ -2936,22 +2960,22 @@
         <v>0.08</v>
       </c>
       <c r="C10">
-        <f>$B$2+$D$2 *(COS((A10+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.2410366037959717E-2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.8098644369496182E-6</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.19262345679012341</v>
       </c>
       <c r="H10">
         <v>-45</v>
       </c>
       <c r="I10">
-        <f>$B$2+0.5*$D$2 *(1+COS((H10+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>8.2410366037959704E-2</v>
       </c>
       <c r="J10">
@@ -2961,7 +2985,7 @@
         <v>-45</v>
       </c>
       <c r="L10">
-        <f>$B$2+$D$2 *(COS((K10+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>8.2410366037959717E-2</v>
       </c>
     </row>
@@ -2973,29 +2997,29 @@
         <v>0.09</v>
       </c>
       <c r="C11">
-        <f>$B$2+$D$2 *(COS((A11+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>9.3069880438561556E-2</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.4241659070629104E-6</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.18394567901234568</v>
       </c>
       <c r="H11">
         <v>-35</v>
       </c>
       <c r="I11">
-        <f>$B$2+0.5*$D$2 *(1+COS((H11+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>9.3069880438561556E-2</v>
       </c>
       <c r="K11">
         <v>-35</v>
       </c>
       <c r="L11">
-        <f>$B$2+$D$2 *(COS((K11+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>9.3069880438561556E-2</v>
       </c>
     </row>
@@ -3007,29 +3031,29 @@
         <v>0.15</v>
       </c>
       <c r="C12">
-        <f>$B$2+$D$2 *(COS((A12+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.15522346807578169</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.7284618738710527E-5</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.13607901234567896</v>
       </c>
       <c r="H12">
         <v>-25</v>
       </c>
       <c r="I12">
-        <f>$B$2+0.5*$D$2 *(1+COS((H12+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.15522346807578169</v>
       </c>
       <c r="K12">
         <v>-25</v>
       </c>
       <c r="L12">
-        <f>$B$2+$D$2 *(COS((K12+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.15522346807578169</v>
       </c>
     </row>
@@ -3041,29 +3065,29 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="C13">
-        <f>$B$2+$D$2 *(COS((A13+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.26137448899131183</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.3144330074119234E-5</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.4459567901234541E-2</v>
       </c>
       <c r="H13">
         <v>-15</v>
       </c>
       <c r="I13">
-        <f>$B$2+0.5*$D$2 *(1+COS((H13+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.26137448899131188</v>
       </c>
       <c r="K13">
         <v>-15</v>
       </c>
       <c r="L13">
-        <f>$B$2+$D$2 *(COS((K13+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.26137448899131183</v>
       </c>
     </row>
@@ -3075,29 +3099,29 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="C14">
-        <f>$B$2+$D$2 *(COS((A14+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.39871956344052045</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.6505261456723759E-4</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.0792901234567895E-2</v>
       </c>
       <c r="H14">
         <v>-5</v>
       </c>
       <c r="I14">
-        <f>$B$2+0.5*$D$2 *(1+COS((H14+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.3987195634405204</v>
       </c>
       <c r="K14">
         <v>-5</v>
       </c>
       <c r="L14">
-        <f>$B$2+$D$2 *(COS((K14+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.39871956344052045</v>
       </c>
     </row>
@@ -3109,29 +3133,29 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="C15">
-        <f>$B$2+$D$2 *(COS((A15+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.55069284844741528</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.601224613418488E-4</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.7345679012346501E-5</v>
       </c>
       <c r="H15">
         <v>5</v>
       </c>
       <c r="I15">
-        <f>$B$2+0.5*$D$2 *(1+COS((H15+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.55069284844741517</v>
       </c>
       <c r="K15">
         <v>5</v>
       </c>
       <c r="L15">
-        <f>$B$2+$D$2 *(COS((K15+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.55069284844741528</v>
       </c>
     </row>
@@ -3143,33 +3167,33 @@
         <v>0.71</v>
       </c>
       <c r="C16">
-        <f>$B$2+$D$2 *(COS((A16+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.69896412295335208</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.2179058218872953E-4</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.6523456790123462E-2</v>
       </c>
       <c r="H16">
         <v>15</v>
       </c>
       <c r="I16">
-        <f>$B$2+0.5*$D$2 *(1+COS((H16+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.69896412295335208</v>
       </c>
       <c r="K16">
         <v>15</v>
       </c>
       <c r="L16">
-        <f>$B$2+$D$2 *(COS((K16+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.69896412295335208</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -3177,33 +3201,33 @@
         <v>0.82</v>
       </c>
       <c r="C17">
-        <f>$B$2+$D$2 *(COS((A17+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.82564968300195885</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.191891802262326E-5</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.0667901234567902E-2</v>
       </c>
       <c r="H17">
         <v>25</v>
       </c>
       <c r="I17">
-        <f>$B$2+0.5*$D$2 *(1+COS((H17+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.82564968300195873</v>
       </c>
       <c r="K17">
         <v>25</v>
       </c>
       <c r="L17">
-        <f>$B$2+$D$2 *(COS((K17+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.82564968300195885</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>35</v>
       </c>
@@ -3211,33 +3235,33 @@
         <v>0.87</v>
       </c>
       <c r="C18">
-        <f>$B$2+$D$2 *(COS((A18+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.9154693803716335</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.0674645513802901E-3</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.12327901234567903</v>
       </c>
       <c r="H18">
         <v>35</v>
       </c>
       <c r="I18">
-        <f>$B$2+0.5*$D$2 *(1+COS((H18+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.9154693803716335</v>
       </c>
       <c r="K18">
         <v>35</v>
       </c>
       <c r="L18">
-        <f>$B$2+$D$2 *(COS((K18+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.9154693803716335</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>45</v>
       </c>
@@ -3245,33 +3269,33 @@
         <v>0.96</v>
       </c>
       <c r="C19">
-        <f>$B$2+$D$2 *(COS((A19+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.95758963396204011</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.8098644369502873E-6</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.19457901234567901</v>
       </c>
       <c r="H19">
         <v>45</v>
       </c>
       <c r="I19">
-        <f>$B$2+0.5*$D$2 *(1+COS((H19+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.95758963396204022</v>
       </c>
       <c r="K19">
         <v>45</v>
       </c>
       <c r="L19">
-        <f>$B$2+$D$2 *(COS((K19+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.95758963396204011</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>55</v>
       </c>
@@ -3279,22 +3303,22 @@
         <v>0.98</v>
       </c>
       <c r="C20">
-        <f>$B$2+$D$2 *(COS((A20+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.94693011956143835</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.093616992220761E-3</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.21262345679012348</v>
       </c>
       <c r="H20">
         <v>55</v>
       </c>
       <c r="I20">
-        <f>$B$2+0.5*$D$2 *(1+COS((H20+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.94693011956143835</v>
       </c>
       <c r="J20">
@@ -3305,11 +3329,11 @@
         <v>55</v>
       </c>
       <c r="L20">
-        <f>$B$2+$D$2 *(COS((K20+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.94693011956143835</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>65</v>
       </c>
@@ -3317,33 +3341,33 @@
         <v>0.88</v>
       </c>
       <c r="C21">
-        <f>$B$2+$D$2 *(COS((A21+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.88477653192421823</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.2815257223075909E-5</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.13040123456790126</v>
       </c>
       <c r="H21">
         <v>65</v>
       </c>
       <c r="I21">
-        <f>$B$2+0.5*$D$2 *(1+COS((H21+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.88477653192421823</v>
       </c>
       <c r="K21">
         <v>65</v>
       </c>
       <c r="L21">
-        <f>$B$2+$D$2 *(COS((K21+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.88477653192421823</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>75</v>
       </c>
@@ -3351,33 +3375,33 @@
         <v>0.78</v>
       </c>
       <c r="C22">
-        <f>$B$2+$D$2 *(COS((A22+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.77862551100868826</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.8892199872372247E-6</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.8179012345679052E-2</v>
       </c>
       <c r="H22">
         <v>75</v>
       </c>
       <c r="I22">
-        <f>$B$2+0.5*$D$2 *(1+COS((H22+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.77862551100868815</v>
       </c>
       <c r="K22">
         <v>75</v>
       </c>
       <c r="L22">
-        <f>$B$2+$D$2 *(COS((K22+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.77862551100868826</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>85</v>
       </c>
@@ -3385,33 +3409,33 @@
         <v>0.66</v>
       </c>
       <c r="C23">
-        <f>$B$2+$D$2 *(COS((A23+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.64128043655947953</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.5042205540367186E-4</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9912345679012369E-2</v>
       </c>
       <c r="H23">
         <v>85</v>
       </c>
       <c r="I23">
-        <f>$B$2+0.5*$D$2 *(1+COS((H23+$A$2)*2*PI()/180))</f>
+        <f t="shared" si="1"/>
         <v>0.64128043655947953</v>
       </c>
       <c r="K23">
         <v>85</v>
       </c>
       <c r="L23">
-        <f>$B$2+$D$2 *(COS((K23+$A$2)*PI()/180)^2)</f>
+        <f t="shared" si="2"/>
         <v>0.64128043655947953</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>8</v>
       </c>
@@ -3419,7 +3443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25">
         <f>AVERAGE(B6:B23)</f>
         <v>0.51888888888888884</v>
@@ -3437,15 +3461,197 @@
         <v>1.745527777777778</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D28">
         <f>1-(D25/E25)</f>
         <v>0.99720257930533396</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>-85</v>
+      </c>
+      <c r="C31">
+        <v>-75</v>
+      </c>
+      <c r="D31">
+        <v>-65</v>
+      </c>
+      <c r="E31">
+        <v>-55</v>
+      </c>
+      <c r="F31">
+        <v>-45</v>
+      </c>
+      <c r="G31">
+        <v>-35</v>
+      </c>
+      <c r="H31">
+        <v>-25</v>
+      </c>
+      <c r="I31">
+        <v>-15</v>
+      </c>
+      <c r="J31">
+        <v>-5</v>
+      </c>
+      <c r="K31">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <v>15</v>
+      </c>
+      <c r="M31">
+        <v>25</v>
+      </c>
+      <c r="N31">
+        <v>35</v>
+      </c>
+      <c r="O31">
+        <v>45</v>
+      </c>
+      <c r="P31">
+        <v>55</v>
+      </c>
+      <c r="Q31">
+        <v>65</v>
+      </c>
+      <c r="R31">
+        <v>75</v>
+      </c>
+      <c r="S31">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="C32">
+        <v>0.34</v>
+      </c>
+      <c r="D32">
+        <v>0.215</v>
+      </c>
+      <c r="E32">
+        <v>0.125</v>
+      </c>
+      <c r="F32">
+        <v>0.08</v>
+      </c>
+      <c r="G32">
+        <v>0.09</v>
+      </c>
+      <c r="H32">
+        <v>0.15</v>
+      </c>
+      <c r="I32">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="J32">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="K32">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="L32">
+        <v>0.71</v>
+      </c>
+      <c r="M32">
+        <v>0.82</v>
+      </c>
+      <c r="N32">
+        <v>0.87</v>
+      </c>
+      <c r="O32">
+        <v>0.96</v>
+      </c>
+      <c r="P32">
+        <v>0.98</v>
+      </c>
+      <c r="Q32">
+        <v>0.88</v>
+      </c>
+      <c r="R32">
+        <v>0.78</v>
+      </c>
+      <c r="S32">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <f>1.1</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37">
+        <f>((D35^2)/2)*(1+(SQRT(2)/2)*SIN(2*E35))</f>
+        <v>0.98745141743001263</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37">
+        <f>E37*(COS(90-$E$35)^2)</f>
+        <v>0.27250024503513615</v>
+      </c>
+      <c r="J37">
+        <v>0.4</v>
+      </c>
+      <c r="K37">
+        <f>J37/J36</f>
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <f>0.5*(D35^2)</f>
+        <v>0.60500000000000009</v>
+      </c>
+      <c r="H38">
+        <f>E38*(COS(90-$E$35)^2)</f>
+        <v>0.16695773112092607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>